<commit_message>
change fields of case officer, inspector, officer to list<text>
</commit_message>
<xml_diff>
--- a/config/field mapping.xlsx
+++ b/config/field mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11160"/>
+    <workbookView windowWidth="20490" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="246">
   <si>
     <t>Column</t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t>Apprehending Officer</t>
+  </si>
+  <si>
+    <t>inspector</t>
   </si>
   <si>
     <t>officer</t>
@@ -756,10 +759,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -813,14 +816,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -830,7 +825,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -843,9 +862,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -867,6 +893,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -882,40 +916,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -929,29 +954,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1020,13 +1023,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1038,7 +1107,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1056,19 +1185,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1081,126 +1204,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1301,6 +1304,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1331,15 +1363,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1351,15 +1374,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1387,31 +1401,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1421,134 +1424,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1618,12 +1621,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1985,10 +1982,10 @@
   <sheetPr/>
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A82" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="E28" sqref="E28"/>
+      <selection pane="topRight" activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2045,10 +2042,10 @@
       <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="26" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2065,8 +2062,8 @@
       <c r="F3" s="18"/>
       <c r="G3" s="19"/>
       <c r="H3" s="20"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="28"/>
     </row>
     <row r="4" ht="15.75" spans="1:10">
       <c r="A4" s="13" t="s">
@@ -2081,8 +2078,8 @@
       <c r="F4" s="18"/>
       <c r="G4" s="19"/>
       <c r="H4" s="20"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="28"/>
     </row>
     <row r="5" ht="15.75" spans="1:10">
       <c r="A5" s="13" t="s">
@@ -2099,8 +2096,8 @@
       <c r="F5" s="18"/>
       <c r="G5" s="19"/>
       <c r="H5" s="20"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="30"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" ht="15.75" spans="1:10">
       <c r="A6" s="13" t="s">
@@ -2119,10 +2116,10 @@
       <c r="H6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="29" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2141,8 +2138,8 @@
       <c r="F7" s="18"/>
       <c r="G7" s="19"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="30"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="28"/>
     </row>
     <row r="8" ht="15.75" spans="1:10">
       <c r="A8" s="13" t="s">
@@ -2163,8 +2160,8 @@
       <c r="F8" s="18"/>
       <c r="G8" s="19"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" ht="15.75" spans="1:10">
       <c r="A9" s="13" t="s">
@@ -2183,8 +2180,8 @@
       <c r="F9" s="18"/>
       <c r="G9" s="19"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
     </row>
     <row r="10" ht="15.75" spans="1:10">
       <c r="A10" s="13" t="s">
@@ -2205,8 +2202,8 @@
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="20"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="30"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
     </row>
     <row r="11" ht="15.75" spans="1:10">
       <c r="A11" s="13" t="s">
@@ -2227,8 +2224,8 @@
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
     </row>
     <row r="12" ht="15.75" spans="1:10">
       <c r="A12" s="13" t="s">
@@ -2249,8 +2246,8 @@
       <c r="F12" s="18"/>
       <c r="G12" s="19"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
     </row>
     <row r="13" ht="15.75" spans="1:10">
       <c r="A13" s="13" t="s">
@@ -2269,8 +2266,8 @@
       <c r="F13" s="18"/>
       <c r="G13" s="19"/>
       <c r="H13" s="20"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="30"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28"/>
     </row>
     <row r="14" ht="15.75" spans="1:10">
       <c r="A14" s="13" t="s">
@@ -2289,8 +2286,8 @@
       <c r="F14" s="18"/>
       <c r="G14" s="19"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
     </row>
     <row r="15" ht="15.75" spans="1:10">
       <c r="A15" s="13" t="s">
@@ -2309,8 +2306,8 @@
       <c r="F15" s="18"/>
       <c r="G15" s="19"/>
       <c r="H15" s="20"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="28"/>
     </row>
     <row r="16" ht="15.75" spans="1:10">
       <c r="A16" s="13" t="s">
@@ -2329,8 +2326,8 @@
       <c r="F16" s="18"/>
       <c r="G16" s="19"/>
       <c r="H16" s="20"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="30"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" ht="15.75" spans="1:10">
       <c r="A17" s="13" t="s">
@@ -2349,8 +2346,8 @@
       <c r="F17" s="18"/>
       <c r="G17" s="19"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="28"/>
     </row>
     <row r="18" ht="15.75" spans="1:10">
       <c r="A18" s="13" t="s">
@@ -2369,8 +2366,8 @@
       <c r="F18" s="18"/>
       <c r="G18" s="19"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="30"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" ht="15.75" spans="1:10">
       <c r="A19" s="13" t="s">
@@ -2389,8 +2386,8 @@
       <c r="F19" s="18"/>
       <c r="G19" s="19"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" ht="15.75" spans="1:10">
       <c r="A20" s="13" t="s">
@@ -2409,8 +2406,8 @@
       <c r="F20" s="18"/>
       <c r="G20" s="19"/>
       <c r="H20" s="20"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21" ht="15.75" spans="1:10">
       <c r="A21" s="13" t="s">
@@ -2429,8 +2426,8 @@
       <c r="F21" s="18"/>
       <c r="G21" s="19"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="30"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
     </row>
     <row r="22" ht="15.75" spans="1:10">
       <c r="A22" s="13" t="s">
@@ -2449,8 +2446,8 @@
       <c r="F22" s="18"/>
       <c r="G22" s="19"/>
       <c r="H22" s="20"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="30"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="28"/>
     </row>
     <row r="23" ht="15.75" spans="1:10">
       <c r="A23" s="13" t="s">
@@ -2469,8 +2466,8 @@
       <c r="F23" s="18"/>
       <c r="G23" s="19"/>
       <c r="H23" s="20"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="30"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="28"/>
     </row>
     <row r="24" ht="15.75" spans="1:10">
       <c r="A24" s="13" t="s">
@@ -2489,8 +2486,8 @@
       <c r="F24" s="18"/>
       <c r="G24" s="19"/>
       <c r="H24" s="20"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="30"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="28"/>
     </row>
     <row r="25" ht="15.75" spans="1:10">
       <c r="A25" s="13" t="s">
@@ -2509,8 +2506,8 @@
       <c r="F25" s="18"/>
       <c r="G25" s="19"/>
       <c r="H25" s="20"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="30"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="28"/>
     </row>
     <row r="26" ht="15.75" spans="1:10">
       <c r="A26" s="13" t="s">
@@ -2529,8 +2526,8 @@
       <c r="F26" s="18"/>
       <c r="G26" s="19"/>
       <c r="H26" s="20"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="30"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="28"/>
     </row>
     <row r="27" ht="15.75" spans="1:10">
       <c r="A27" s="13" t="s">
@@ -2549,8 +2546,8 @@
       <c r="F27" s="18"/>
       <c r="G27" s="19"/>
       <c r="H27" s="20"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="30"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" ht="15.75" spans="1:10">
       <c r="A28" s="13" t="s">
@@ -2567,8 +2564,8 @@
       <c r="F28" s="18"/>
       <c r="G28" s="19"/>
       <c r="H28" s="20"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="30"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" ht="15.75" spans="1:10">
       <c r="A29" s="13" t="s">
@@ -2585,8 +2582,8 @@
       <c r="F29" s="18"/>
       <c r="G29" s="19"/>
       <c r="H29" s="20"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="30"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="28"/>
     </row>
     <row r="30" ht="15.75" spans="1:10">
       <c r="A30" s="13" t="s">
@@ -2603,8 +2600,8 @@
       <c r="F30" s="18"/>
       <c r="G30" s="19"/>
       <c r="H30" s="20"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="28"/>
     </row>
     <row r="31" ht="15.75" spans="1:10">
       <c r="A31" s="13" t="s">
@@ -2621,8 +2618,8 @@
       <c r="F31" s="18"/>
       <c r="G31" s="19"/>
       <c r="H31" s="20"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="30"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="28"/>
     </row>
     <row r="32" ht="15.75" spans="1:10">
       <c r="A32" s="13" t="s">
@@ -2639,8 +2636,8 @@
       <c r="F32" s="18"/>
       <c r="G32" s="19"/>
       <c r="H32" s="20"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="30"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" ht="15.75" spans="1:10">
       <c r="A33" s="13" t="s">
@@ -2657,8 +2654,8 @@
       <c r="F33" s="18"/>
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="30"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="28"/>
     </row>
     <row r="34" ht="15.75" spans="1:10">
       <c r="A34" s="13" t="s">
@@ -2675,8 +2672,8 @@
       <c r="F34" s="18"/>
       <c r="G34" s="19"/>
       <c r="H34" s="20"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="30"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="28"/>
     </row>
     <row r="35" ht="15.75" spans="1:10">
       <c r="A35" s="13" t="s">
@@ -2693,8 +2690,8 @@
       <c r="F35" s="18"/>
       <c r="G35" s="19"/>
       <c r="H35" s="20"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="30"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="28"/>
     </row>
     <row r="36" ht="15.75" spans="1:10">
       <c r="A36" s="13" t="s">
@@ -2711,8 +2708,8 @@
       <c r="F36" s="18"/>
       <c r="G36" s="19"/>
       <c r="H36" s="20"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="30"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="28"/>
     </row>
     <row r="37" ht="15.75" spans="1:10">
       <c r="A37" s="13" t="s">
@@ -2729,8 +2726,8 @@
       <c r="F37" s="18"/>
       <c r="G37" s="19"/>
       <c r="H37" s="20"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="30"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="28"/>
     </row>
     <row r="38" ht="15.75" spans="1:10">
       <c r="A38" s="13" t="s">
@@ -2747,8 +2744,8 @@
       <c r="F38" s="18"/>
       <c r="G38" s="19"/>
       <c r="H38" s="20"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="30"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="28"/>
     </row>
     <row r="39" ht="15.75" spans="1:10">
       <c r="A39" s="13" t="s">
@@ -2765,8 +2762,8 @@
       <c r="F39" s="18"/>
       <c r="G39" s="19"/>
       <c r="H39" s="20"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="30"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="28"/>
     </row>
     <row r="40" ht="15.75" spans="1:10">
       <c r="A40" s="13" t="s">
@@ -2783,8 +2780,8 @@
       <c r="F40" s="18"/>
       <c r="G40" s="19"/>
       <c r="H40" s="20"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="30"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="28"/>
     </row>
     <row r="41" ht="15.75" spans="1:10">
       <c r="A41" s="13" t="s">
@@ -2801,8 +2798,8 @@
       <c r="F41" s="18"/>
       <c r="G41" s="19"/>
       <c r="H41" s="20"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="30"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="28"/>
     </row>
     <row r="42" ht="15.75" spans="1:10">
       <c r="A42" s="13" t="s">
@@ -2819,8 +2816,8 @@
       <c r="F42" s="18"/>
       <c r="G42" s="19"/>
       <c r="H42" s="20"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="28"/>
     </row>
     <row r="43" ht="15.75" spans="1:10">
       <c r="A43" s="13" t="s">
@@ -2837,8 +2834,8 @@
       <c r="F43" s="18"/>
       <c r="G43" s="19"/>
       <c r="H43" s="20"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="28"/>
     </row>
     <row r="44" ht="15.75" spans="1:10">
       <c r="A44" s="13" t="s">
@@ -2855,8 +2852,8 @@
       <c r="F44" s="18"/>
       <c r="G44" s="19"/>
       <c r="H44" s="20"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="30"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="28"/>
     </row>
     <row r="45" ht="15.75" spans="1:10">
       <c r="A45" s="13" t="s">
@@ -2873,8 +2870,8 @@
       <c r="F45" s="18"/>
       <c r="G45" s="19"/>
       <c r="H45" s="20"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="28"/>
     </row>
     <row r="46" ht="15.75" spans="1:10">
       <c r="A46" s="13" t="s">
@@ -2891,8 +2888,8 @@
       <c r="F46" s="18"/>
       <c r="G46" s="19"/>
       <c r="H46" s="20"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="28"/>
     </row>
     <row r="47" ht="15.75" spans="1:10">
       <c r="A47" s="13" t="s">
@@ -2909,8 +2906,8 @@
       <c r="F47" s="18"/>
       <c r="G47" s="19"/>
       <c r="H47" s="20"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="30"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="28"/>
     </row>
     <row r="48" ht="15.75" spans="1:10">
       <c r="A48" s="13" t="s">
@@ -2927,8 +2924,8 @@
       <c r="F48" s="18"/>
       <c r="G48" s="19"/>
       <c r="H48" s="20"/>
-      <c r="I48" s="29"/>
-      <c r="J48" s="30"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="28"/>
     </row>
     <row r="49" ht="15.75" spans="1:10">
       <c r="A49" s="13" t="s">
@@ -2945,8 +2942,8 @@
       <c r="F49" s="18"/>
       <c r="G49" s="19"/>
       <c r="H49" s="20"/>
-      <c r="I49" s="29"/>
-      <c r="J49" s="30"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="28"/>
     </row>
     <row r="50" ht="15.75" spans="1:10">
       <c r="A50" s="13" t="s">
@@ -2963,8 +2960,8 @@
       <c r="F50" s="18"/>
       <c r="G50" s="19"/>
       <c r="H50" s="20"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="30"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="28"/>
     </row>
     <row r="51" ht="15.75" spans="1:10">
       <c r="A51" s="13" t="s">
@@ -2981,8 +2978,8 @@
       <c r="F51" s="18"/>
       <c r="G51" s="19"/>
       <c r="H51" s="20"/>
-      <c r="I51" s="29"/>
-      <c r="J51" s="30"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="28"/>
     </row>
     <row r="52" ht="15.75" spans="1:10">
       <c r="A52" s="13" t="s">
@@ -2999,8 +2996,8 @@
       <c r="F52" s="18"/>
       <c r="G52" s="19"/>
       <c r="H52" s="20"/>
-      <c r="I52" s="29"/>
-      <c r="J52" s="30"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="28"/>
     </row>
     <row r="53" ht="15.75" spans="1:10">
       <c r="A53" s="13" t="s">
@@ -3017,8 +3014,8 @@
       <c r="F53" s="18"/>
       <c r="G53" s="19"/>
       <c r="H53" s="20"/>
-      <c r="I53" s="29"/>
-      <c r="J53" s="30"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="28"/>
     </row>
     <row r="54" ht="15.75" spans="1:10">
       <c r="A54" s="13" t="s">
@@ -3035,8 +3032,8 @@
       <c r="F54" s="18"/>
       <c r="G54" s="19"/>
       <c r="H54" s="20"/>
-      <c r="I54" s="29"/>
-      <c r="J54" s="30"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="28"/>
     </row>
     <row r="55" ht="15.75" spans="1:10">
       <c r="A55" s="13" t="s">
@@ -3053,8 +3050,8 @@
       <c r="F55" s="18"/>
       <c r="G55" s="19"/>
       <c r="H55" s="20"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="30"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="28"/>
     </row>
     <row r="56" ht="15.75" spans="1:10">
       <c r="A56" s="13" t="s">
@@ -3071,8 +3068,8 @@
       <c r="F56" s="18"/>
       <c r="G56" s="19"/>
       <c r="H56" s="20"/>
-      <c r="I56" s="29"/>
-      <c r="J56" s="30"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="28"/>
     </row>
     <row r="57" ht="15.75" spans="1:10">
       <c r="A57" s="13" t="s">
@@ -3089,8 +3086,8 @@
       <c r="F57" s="18"/>
       <c r="G57" s="19"/>
       <c r="H57" s="20"/>
-      <c r="I57" s="29"/>
-      <c r="J57" s="30"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="28"/>
     </row>
     <row r="58" ht="15.75" spans="1:10">
       <c r="A58" s="13" t="s">
@@ -3105,8 +3102,8 @@
       <c r="F58" s="18"/>
       <c r="G58" s="19"/>
       <c r="H58" s="20"/>
-      <c r="I58" s="29"/>
-      <c r="J58" s="30"/>
+      <c r="I58" s="27"/>
+      <c r="J58" s="28"/>
     </row>
     <row r="59" ht="15.75" spans="1:10">
       <c r="A59" s="13" t="s">
@@ -3120,11 +3117,11 @@
       <c r="E59" s="17"/>
       <c r="F59" s="18"/>
       <c r="G59" s="19"/>
-      <c r="H59" s="24" t="s">
+      <c r="H59" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="I59" s="29"/>
-      <c r="J59" s="30"/>
+      <c r="I59" s="27"/>
+      <c r="J59" s="28"/>
     </row>
     <row r="60" ht="15.75" spans="1:10">
       <c r="A60" s="13" t="s">
@@ -3138,11 +3135,11 @@
       <c r="E60" s="17"/>
       <c r="F60" s="18"/>
       <c r="G60" s="19"/>
-      <c r="H60" s="25" t="s">
+      <c r="H60" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="I60" s="29"/>
-      <c r="J60" s="30"/>
+      <c r="I60" s="27"/>
+      <c r="J60" s="28"/>
     </row>
     <row r="61" ht="15.75" spans="1:10">
       <c r="A61" s="13" t="s">
@@ -3156,9 +3153,9 @@
       <c r="E61" s="17"/>
       <c r="F61" s="18"/>
       <c r="G61" s="19"/>
-      <c r="H61" s="25"/>
-      <c r="I61" s="29"/>
-      <c r="J61" s="30"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="28"/>
     </row>
     <row r="62" ht="15.75" spans="1:10">
       <c r="A62" s="13" t="s">
@@ -3172,11 +3169,11 @@
       <c r="E62" s="17"/>
       <c r="F62" s="18"/>
       <c r="G62" s="19"/>
-      <c r="H62" s="24" t="s">
+      <c r="H62" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="I62" s="29"/>
-      <c r="J62" s="30"/>
+      <c r="I62" s="27"/>
+      <c r="J62" s="28"/>
     </row>
     <row r="63" ht="15.75" spans="1:10">
       <c r="A63" s="13" t="s">
@@ -3190,17 +3187,17 @@
       <c r="E63" s="17"/>
       <c r="F63" s="18"/>
       <c r="G63" s="19"/>
-      <c r="H63" s="24" t="s">
+      <c r="H63" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="I63" s="29"/>
-      <c r="J63" s="30"/>
+      <c r="I63" s="27"/>
+      <c r="J63" s="28"/>
     </row>
     <row r="64" ht="15.75" spans="1:10">
       <c r="A64" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B64" s="26" t="s">
+      <c r="B64" s="24" t="s">
         <v>147</v>
       </c>
       <c r="C64" s="15"/>
@@ -3208,11 +3205,11 @@
       <c r="E64" s="17"/>
       <c r="F64" s="18"/>
       <c r="G64" s="19"/>
-      <c r="H64" s="24" t="s">
+      <c r="H64" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="I64" s="29"/>
-      <c r="J64" s="30"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="28"/>
     </row>
     <row r="65" ht="15.75" spans="1:10">
       <c r="A65" s="13" t="s">
@@ -3226,11 +3223,11 @@
       <c r="E65" s="17"/>
       <c r="F65" s="18"/>
       <c r="G65" s="19"/>
-      <c r="H65" s="24" t="s">
+      <c r="H65" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="I65" s="29"/>
-      <c r="J65" s="30"/>
+      <c r="I65" s="27"/>
+      <c r="J65" s="28"/>
     </row>
     <row r="66" ht="15.75" spans="1:10">
       <c r="A66" s="13" t="s">
@@ -3244,11 +3241,11 @@
       <c r="E66" s="17"/>
       <c r="F66" s="18"/>
       <c r="G66" s="19"/>
-      <c r="H66" s="25" t="s">
+      <c r="H66" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="I66" s="29"/>
-      <c r="J66" s="30"/>
+      <c r="I66" s="27"/>
+      <c r="J66" s="28"/>
     </row>
     <row r="67" ht="15.75" spans="1:10">
       <c r="A67" s="13" t="s">
@@ -3262,9 +3259,9 @@
       <c r="E67" s="17"/>
       <c r="F67" s="18"/>
       <c r="G67" s="19"/>
-      <c r="H67" s="25"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="30"/>
+      <c r="H67" s="20"/>
+      <c r="I67" s="27"/>
+      <c r="J67" s="28"/>
     </row>
     <row r="68" ht="15.75" spans="1:10">
       <c r="A68" s="13" t="s">
@@ -3278,11 +3275,11 @@
       <c r="E68" s="17"/>
       <c r="F68" s="18"/>
       <c r="G68" s="19"/>
-      <c r="H68" s="24" t="s">
+      <c r="H68" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="I68" s="29"/>
-      <c r="J68" s="30"/>
+      <c r="I68" s="27"/>
+      <c r="J68" s="28"/>
     </row>
     <row r="69" ht="15.75" spans="1:10">
       <c r="A69" s="13" t="s">
@@ -3296,11 +3293,11 @@
       <c r="E69" s="17"/>
       <c r="F69" s="18"/>
       <c r="G69" s="19"/>
-      <c r="H69" s="25" t="s">
+      <c r="H69" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="I69" s="29"/>
-      <c r="J69" s="30"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="28"/>
     </row>
     <row r="70" ht="15.75" spans="1:10">
       <c r="A70" s="13" t="s">
@@ -3314,9 +3311,9 @@
       <c r="E70" s="17"/>
       <c r="F70" s="18"/>
       <c r="G70" s="19"/>
-      <c r="H70" s="25"/>
-      <c r="I70" s="29"/>
-      <c r="J70" s="30"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="27"/>
+      <c r="J70" s="28"/>
     </row>
     <row r="71" ht="15.75" spans="1:10">
       <c r="A71" s="13" t="s">
@@ -3330,11 +3327,11 @@
       <c r="E71" s="17"/>
       <c r="F71" s="18"/>
       <c r="G71" s="19"/>
-      <c r="H71" s="24" t="s">
+      <c r="H71" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="I71" s="29"/>
-      <c r="J71" s="30"/>
+      <c r="I71" s="27"/>
+      <c r="J71" s="28"/>
     </row>
     <row r="72" ht="15.75" spans="1:10">
       <c r="A72" s="13" t="s">
@@ -3348,11 +3345,11 @@
       <c r="E72" s="17"/>
       <c r="F72" s="18"/>
       <c r="G72" s="19"/>
-      <c r="H72" s="25" t="s">
+      <c r="H72" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="I72" s="29"/>
-      <c r="J72" s="30"/>
+      <c r="I72" s="27"/>
+      <c r="J72" s="28"/>
     </row>
     <row r="73" ht="15.75" spans="1:10">
       <c r="A73" s="13" t="s">
@@ -3366,9 +3363,9 @@
       <c r="E73" s="17"/>
       <c r="F73" s="18"/>
       <c r="G73" s="19"/>
-      <c r="H73" s="25"/>
-      <c r="I73" s="29"/>
-      <c r="J73" s="30"/>
+      <c r="H73" s="20"/>
+      <c r="I73" s="27"/>
+      <c r="J73" s="28"/>
     </row>
     <row r="74" ht="15.75" spans="1:10">
       <c r="A74" s="13" t="s">
@@ -3383,10 +3380,10 @@
       <c r="F74" s="18"/>
       <c r="G74" s="19"/>
       <c r="H74" s="20"/>
-      <c r="I74" s="36" t="s">
+      <c r="I74" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="J74" s="30"/>
+      <c r="J74" s="28"/>
     </row>
     <row r="75" ht="15.75" spans="1:10">
       <c r="A75" s="13" t="s">
@@ -3401,10 +3398,10 @@
       <c r="F75" s="18"/>
       <c r="G75" s="19"/>
       <c r="H75" s="20"/>
-      <c r="I75" s="36" t="s">
+      <c r="I75" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="J75" s="30"/>
+      <c r="J75" s="28"/>
     </row>
     <row r="76" ht="15.75" spans="1:10">
       <c r="A76" s="13" t="s">
@@ -3419,10 +3416,10 @@
       <c r="F76" s="18"/>
       <c r="G76" s="19"/>
       <c r="H76" s="20"/>
-      <c r="I76" s="36" t="s">
+      <c r="I76" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="J76" s="30"/>
+      <c r="J76" s="28"/>
     </row>
     <row r="77" ht="15.75" spans="1:10">
       <c r="A77" s="13" t="s">
@@ -3437,10 +3434,10 @@
       <c r="F77" s="18"/>
       <c r="G77" s="19"/>
       <c r="H77" s="20"/>
-      <c r="I77" s="36" t="s">
+      <c r="I77" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="J77" s="30"/>
+      <c r="J77" s="28"/>
     </row>
     <row r="78" ht="15.75" spans="1:10">
       <c r="A78" s="13" t="s">
@@ -3455,10 +3452,10 @@
       <c r="F78" s="18"/>
       <c r="G78" s="19"/>
       <c r="H78" s="20"/>
-      <c r="I78" s="36" t="s">
+      <c r="I78" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="J78" s="30"/>
+      <c r="J78" s="28"/>
     </row>
     <row r="79" ht="15.75" spans="1:10">
       <c r="A79" s="13" t="s">
@@ -3473,10 +3470,10 @@
       <c r="F79" s="18"/>
       <c r="G79" s="19"/>
       <c r="H79" s="20"/>
-      <c r="I79" s="36" t="s">
+      <c r="I79" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="J79" s="30"/>
+      <c r="J79" s="28"/>
     </row>
     <row r="80" ht="15.75" spans="1:10">
       <c r="A80" s="13" t="s">
@@ -3491,10 +3488,10 @@
       <c r="F80" s="18"/>
       <c r="G80" s="19"/>
       <c r="H80" s="20"/>
-      <c r="I80" s="29" t="s">
+      <c r="I80" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="J80" s="30"/>
+      <c r="J80" s="28"/>
     </row>
     <row r="81" ht="15.75" spans="1:10">
       <c r="A81" s="13" t="s">
@@ -3509,8 +3506,8 @@
       <c r="F81" s="18"/>
       <c r="G81" s="19"/>
       <c r="H81" s="20"/>
-      <c r="I81" s="29"/>
-      <c r="J81" s="30"/>
+      <c r="I81" s="27"/>
+      <c r="J81" s="28"/>
     </row>
     <row r="82" ht="15.75" spans="1:10">
       <c r="A82" s="13" t="s">
@@ -3525,8 +3522,8 @@
       <c r="F82" s="18"/>
       <c r="G82" s="19"/>
       <c r="H82" s="20"/>
-      <c r="I82" s="29"/>
-      <c r="J82" s="30" t="s">
+      <c r="I82" s="27"/>
+      <c r="J82" s="28" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3543,8 +3540,8 @@
       <c r="F83" s="18"/>
       <c r="G83" s="19"/>
       <c r="H83" s="20"/>
-      <c r="I83" s="29"/>
-      <c r="J83" s="30" t="s">
+      <c r="I83" s="27"/>
+      <c r="J83" s="28" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3561,8 +3558,8 @@
       <c r="F84" s="18"/>
       <c r="G84" s="19"/>
       <c r="H84" s="20"/>
-      <c r="I84" s="29"/>
-      <c r="J84" s="30" t="s">
+      <c r="I84" s="27"/>
+      <c r="J84" s="28" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3579,8 +3576,8 @@
       <c r="F85" s="18"/>
       <c r="G85" s="19"/>
       <c r="H85" s="20"/>
-      <c r="I85" s="29"/>
-      <c r="J85" s="30" t="s">
+      <c r="I85" s="27"/>
+      <c r="J85" s="28" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3597,8 +3594,8 @@
       <c r="F86" s="18"/>
       <c r="G86" s="19"/>
       <c r="H86" s="20"/>
-      <c r="I86" s="29"/>
-      <c r="J86" s="30" t="s">
+      <c r="I86" s="27"/>
+      <c r="J86" s="28" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3615,8 +3612,8 @@
       <c r="F87" s="18"/>
       <c r="G87" s="19"/>
       <c r="H87" s="20"/>
-      <c r="I87" s="29"/>
-      <c r="J87" s="30" t="s">
+      <c r="I87" s="27"/>
+      <c r="J87" s="28" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3633,8 +3630,8 @@
       <c r="F88" s="18"/>
       <c r="G88" s="19"/>
       <c r="H88" s="20"/>
-      <c r="I88" s="29"/>
-      <c r="J88" s="30" t="s">
+      <c r="I88" s="27"/>
+      <c r="J88" s="28" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3651,8 +3648,8 @@
       <c r="F89" s="18"/>
       <c r="G89" s="19"/>
       <c r="H89" s="20"/>
-      <c r="I89" s="29"/>
-      <c r="J89" s="30" t="s">
+      <c r="I89" s="27"/>
+      <c r="J89" s="28" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3669,8 +3666,8 @@
       <c r="F90" s="18"/>
       <c r="G90" s="19"/>
       <c r="H90" s="20"/>
-      <c r="I90" s="29"/>
-      <c r="J90" s="30" t="s">
+      <c r="I90" s="27"/>
+      <c r="J90" s="28" t="s">
         <v>199</v>
       </c>
     </row>
@@ -3687,8 +3684,8 @@
       <c r="F91" s="18"/>
       <c r="G91" s="19"/>
       <c r="H91" s="20"/>
-      <c r="I91" s="29"/>
-      <c r="J91" s="30" t="s">
+      <c r="I91" s="27"/>
+      <c r="J91" s="28" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3709,10 +3706,10 @@
       <c r="H92" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="I92" s="29" t="s">
+      <c r="I92" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="J92" s="31" t="s">
+      <c r="J92" s="29" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3735,10 +3732,10 @@
       <c r="H93" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="I93" s="29" t="s">
+      <c r="I93" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="J93" s="31" t="s">
+      <c r="J93" s="29" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3757,8 +3754,8 @@
       </c>
       <c r="G94" s="19"/>
       <c r="H94" s="20"/>
-      <c r="I94" s="29"/>
-      <c r="J94" s="30"/>
+      <c r="I94" s="27"/>
+      <c r="J94" s="28"/>
     </row>
     <row r="95" ht="15.75" spans="1:10">
       <c r="A95" s="13" t="s">
@@ -3773,8 +3770,8 @@
       <c r="F95" s="18"/>
       <c r="G95" s="19"/>
       <c r="H95" s="20"/>
-      <c r="I95" s="29"/>
-      <c r="J95" s="30"/>
+      <c r="I95" s="27"/>
+      <c r="J95" s="28"/>
     </row>
     <row r="96" ht="15.75" spans="1:10">
       <c r="A96" s="13" t="s">
@@ -3789,8 +3786,8 @@
       <c r="F96" s="18"/>
       <c r="G96" s="19"/>
       <c r="H96" s="20"/>
-      <c r="I96" s="29"/>
-      <c r="J96" s="30"/>
+      <c r="I96" s="27"/>
+      <c r="J96" s="28"/>
     </row>
     <row r="97" ht="15.75" spans="1:10">
       <c r="A97" s="13" t="s">
@@ -3807,8 +3804,8 @@
         <v>218</v>
       </c>
       <c r="H97" s="20"/>
-      <c r="I97" s="29"/>
-      <c r="J97" s="30"/>
+      <c r="I97" s="27"/>
+      <c r="J97" s="28"/>
     </row>
     <row r="98" ht="15.75" spans="1:10">
       <c r="A98" s="13" t="s">
@@ -3825,8 +3822,8 @@
         <v>220</v>
       </c>
       <c r="H98" s="20"/>
-      <c r="I98" s="29"/>
-      <c r="J98" s="30"/>
+      <c r="I98" s="27"/>
+      <c r="J98" s="28"/>
     </row>
     <row r="99" ht="15.75" spans="1:10">
       <c r="A99" s="13" t="s">
@@ -3841,8 +3838,8 @@
       <c r="F99" s="18"/>
       <c r="G99" s="19"/>
       <c r="H99" s="20"/>
-      <c r="I99" s="29"/>
-      <c r="J99" s="30"/>
+      <c r="I99" s="27"/>
+      <c r="J99" s="28"/>
     </row>
     <row r="100" ht="15.75" spans="1:10">
       <c r="A100" s="13" t="s">
@@ -3857,8 +3854,8 @@
       <c r="F100" s="18"/>
       <c r="G100" s="19"/>
       <c r="H100" s="20"/>
-      <c r="I100" s="29"/>
-      <c r="J100" s="30"/>
+      <c r="I100" s="27"/>
+      <c r="J100" s="28"/>
     </row>
     <row r="101" ht="15.75" spans="1:10">
       <c r="A101" s="13" t="s">
@@ -3875,8 +3872,8 @@
         <v>225</v>
       </c>
       <c r="H101" s="20"/>
-      <c r="I101" s="29"/>
-      <c r="J101" s="30"/>
+      <c r="I101" s="27"/>
+      <c r="J101" s="28"/>
     </row>
     <row r="102" ht="15.75" spans="1:10">
       <c r="A102" s="13" t="s">
@@ -3888,134 +3885,136 @@
       <c r="C102" s="15"/>
       <c r="D102" s="16"/>
       <c r="E102" s="17"/>
-      <c r="F102" s="18"/>
+      <c r="F102" s="18" t="s">
+        <v>228</v>
+      </c>
       <c r="G102" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H102" s="20"/>
-      <c r="I102" s="29"/>
-      <c r="J102" s="30"/>
+      <c r="I102" s="27"/>
+      <c r="J102" s="28"/>
     </row>
     <row r="103" ht="15.75" spans="1:10">
       <c r="A103" s="13" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C103" s="15"/>
       <c r="D103" s="16"/>
       <c r="E103" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F103" s="18"/>
       <c r="G103" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H103" s="20"/>
-      <c r="I103" s="29"/>
-      <c r="J103" s="30"/>
+      <c r="I103" s="27"/>
+      <c r="J103" s="28"/>
     </row>
     <row r="104" ht="15.75" spans="1:10">
       <c r="A104" s="13" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C104" s="15"/>
       <c r="D104" s="16"/>
       <c r="E104" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F104" s="18"/>
       <c r="G104" s="19"/>
       <c r="H104" s="20"/>
-      <c r="I104" s="29"/>
-      <c r="J104" s="30"/>
+      <c r="I104" s="27"/>
+      <c r="J104" s="28"/>
     </row>
     <row r="105" ht="15.75" spans="1:10">
       <c r="A105" s="13" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C105" s="15"/>
       <c r="D105" s="16"/>
       <c r="E105" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F105" s="18"/>
       <c r="G105" s="19"/>
       <c r="H105" s="20"/>
-      <c r="I105" s="29"/>
-      <c r="J105" s="30"/>
+      <c r="I105" s="27"/>
+      <c r="J105" s="28"/>
     </row>
     <row r="106" ht="15.75" spans="1:10">
       <c r="A106" s="13" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C106" s="15"/>
       <c r="D106" s="16"/>
       <c r="E106" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F106" s="18"/>
       <c r="G106" s="19" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H106" s="20"/>
-      <c r="I106" s="29"/>
-      <c r="J106" s="30"/>
+      <c r="I106" s="27"/>
+      <c r="J106" s="28"/>
     </row>
     <row r="107" ht="15.75" spans="1:10">
       <c r="A107" s="13" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B107" s="21" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C107" s="15"/>
       <c r="D107" s="16"/>
       <c r="E107" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F107" s="18"/>
-      <c r="G107" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="H107" s="33"/>
-      <c r="I107" s="37"/>
-      <c r="J107" s="38"/>
+      <c r="G107" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="H107" s="31"/>
+      <c r="I107" s="35"/>
+      <c r="J107" s="36"/>
     </row>
     <row r="108" ht="15.75" spans="1:10">
       <c r="A108" s="13"/>
       <c r="B108" s="21"/>
       <c r="C108" s="15"/>
       <c r="D108" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="F108" s="34" t="s">
-        <v>243</v>
-      </c>
-      <c r="G108" s="35" t="s">
-        <v>243</v>
+        <v>244</v>
+      </c>
+      <c r="F108" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="G108" s="33" t="s">
+        <v>244</v>
       </c>
       <c r="H108" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="I108" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="J108" s="31" t="s">
-        <v>243</v>
+        <v>244</v>
+      </c>
+      <c r="I108" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="J108" s="29" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="109" ht="15.75" spans="1:10">
@@ -4023,25 +4022,25 @@
       <c r="B109" s="21"/>
       <c r="C109" s="15"/>
       <c r="D109" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="F109" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="G109" s="35" t="s">
-        <v>244</v>
+        <v>245</v>
+      </c>
+      <c r="F109" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="G109" s="33" t="s">
+        <v>245</v>
       </c>
       <c r="H109" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="I109" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="J109" s="31" t="s">
-        <v>244</v>
+        <v>245</v>
+      </c>
+      <c r="I109" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="J109" s="29" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>